<commit_message>
multi quote and all rule engile financer added
</commit_message>
<xml_diff>
--- a/resource/testdata.xlsx
+++ b/resource/testdata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7210" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9786" uniqueCount="106">
   <si>
     <t>testdata</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>Toyota Avanza Avanza 1.3E MT</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1422,7 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2">

</xml_diff>